<commit_message>
Ajuste da apresentacao, dados novos
</commit_message>
<xml_diff>
--- a/dadosConnepi.xlsx
+++ b/dadosConnepi.xlsx
@@ -8,24 +8,53 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/b7beb5d6fee94c27/Documents/meusCursos/regressao-connepi2024Local/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="11_94B1572A54DEAC0FFB039038BE0E4ED8A2FF9F7C" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F29CF14F-BEA6-4029-8BB6-BC8FF88269E6}"/>
+  <xr:revisionPtr revIDLastSave="30" documentId="11_94B1572A54DEAC0FFB039038BE0E4ED8A2FF9F7C" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{965AD81C-E261-4B4E-8196-A65E7290B9A0}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ex1_compressao" sheetId="1" r:id="rId1"/>
+    <sheet name="ex2_fabrica" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>rca</t>
   </si>
   <si>
     <t>ps</t>
+  </si>
+  <si>
+    <t>data</t>
+  </si>
+  <si>
+    <t>ci</t>
+  </si>
+  <si>
+    <t>toneladas</t>
+  </si>
+  <si>
+    <t>embalagem</t>
+  </si>
+  <si>
+    <t>divugacao</t>
   </si>
 </sst>
 </file>
@@ -78,6 +107,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -361,7 +394,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
@@ -499,4 +532,549 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99824CB9-6BCB-4F57-882F-B49BF57D3479}">
+  <dimension ref="A1:E31"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G20" sqref="G20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="3" max="3" width="10.44140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>42005</v>
+      </c>
+      <c r="B2">
+        <v>218500.95</v>
+      </c>
+      <c r="C2">
+        <v>2790.9</v>
+      </c>
+      <c r="D2">
+        <v>42.3</v>
+      </c>
+      <c r="E2">
+        <v>253.81</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>42036</v>
+      </c>
+      <c r="B3">
+        <v>209982.3</v>
+      </c>
+      <c r="C3">
+        <v>2866.5</v>
+      </c>
+      <c r="D3">
+        <v>29.7</v>
+      </c>
+      <c r="E3">
+        <v>877.03</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>42064</v>
+      </c>
+      <c r="B4">
+        <v>228401.85</v>
+      </c>
+      <c r="C4">
+        <v>2573.5500000000002</v>
+      </c>
+      <c r="D4">
+        <v>53.1</v>
+      </c>
+      <c r="E4">
+        <v>575.83000000000004</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>42095</v>
+      </c>
+      <c r="B5">
+        <v>176657.25</v>
+      </c>
+      <c r="C5">
+        <v>1584.45</v>
+      </c>
+      <c r="D5">
+        <v>54</v>
+      </c>
+      <c r="E5">
+        <v>909.86</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>42125</v>
+      </c>
+      <c r="B6">
+        <v>207152.25</v>
+      </c>
+      <c r="C6">
+        <v>2178.75</v>
+      </c>
+      <c r="D6">
+        <v>53.1</v>
+      </c>
+      <c r="E6">
+        <v>1178.07</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>42156</v>
+      </c>
+      <c r="B7">
+        <v>249873.75</v>
+      </c>
+      <c r="C7">
+        <v>3082.8</v>
+      </c>
+      <c r="D7">
+        <v>55.8</v>
+      </c>
+      <c r="E7">
+        <v>1025.1099999999999</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>42186</v>
+      </c>
+      <c r="B8">
+        <v>223582.5</v>
+      </c>
+      <c r="C8">
+        <v>2459.1</v>
+      </c>
+      <c r="D8">
+        <v>64.8</v>
+      </c>
+      <c r="E8">
+        <v>89.58</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>42217</v>
+      </c>
+      <c r="B9">
+        <v>201306.9</v>
+      </c>
+      <c r="C9">
+        <v>2305.8000000000002</v>
+      </c>
+      <c r="D9">
+        <v>45.9</v>
+      </c>
+      <c r="E9">
+        <v>2075.9499999999998</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>42248</v>
+      </c>
+      <c r="B10">
+        <v>180738.45</v>
+      </c>
+      <c r="C10">
+        <v>2433.9</v>
+      </c>
+      <c r="D10">
+        <v>34.200000000000003</v>
+      </c>
+      <c r="E10">
+        <v>665.05</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>42278</v>
+      </c>
+      <c r="B11">
+        <v>159762.45000000001</v>
+      </c>
+      <c r="C11">
+        <v>1762.95</v>
+      </c>
+      <c r="D11">
+        <v>39.6</v>
+      </c>
+      <c r="E11">
+        <v>2266.21</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>42309</v>
+      </c>
+      <c r="B12">
+        <v>192221.1</v>
+      </c>
+      <c r="C12">
+        <v>2176.65</v>
+      </c>
+      <c r="D12">
+        <v>47.7</v>
+      </c>
+      <c r="E12">
+        <v>1136.08</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>42339</v>
+      </c>
+      <c r="B13">
+        <v>205490.7</v>
+      </c>
+      <c r="C13">
+        <v>2079</v>
+      </c>
+      <c r="D13">
+        <v>63.9</v>
+      </c>
+      <c r="E13">
+        <v>1770.01</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>42370</v>
+      </c>
+      <c r="B14">
+        <v>195319.05</v>
+      </c>
+      <c r="C14">
+        <v>1990.8</v>
+      </c>
+      <c r="D14">
+        <v>66.599999999999994</v>
+      </c>
+      <c r="E14">
+        <v>1259.9100000000001</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>42401</v>
+      </c>
+      <c r="B15">
+        <v>196875.15</v>
+      </c>
+      <c r="C15">
+        <v>2116.8000000000002</v>
+      </c>
+      <c r="D15">
+        <v>39.6</v>
+      </c>
+      <c r="E15">
+        <v>913.48</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>42430</v>
+      </c>
+      <c r="B16">
+        <v>243817.5</v>
+      </c>
+      <c r="C16">
+        <v>2840.25</v>
+      </c>
+      <c r="D16">
+        <v>64.8</v>
+      </c>
+      <c r="E16">
+        <v>604.01</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>42461</v>
+      </c>
+      <c r="B17">
+        <v>165861.45000000001</v>
+      </c>
+      <c r="C17">
+        <v>1609.65</v>
+      </c>
+      <c r="D17">
+        <v>51.3</v>
+      </c>
+      <c r="E17">
+        <v>925.41</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>42491</v>
+      </c>
+      <c r="B18">
+        <v>175634.1</v>
+      </c>
+      <c r="C18">
+        <v>2378.25</v>
+      </c>
+      <c r="D18">
+        <v>28.8</v>
+      </c>
+      <c r="E18">
+        <v>52.24</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>42522</v>
+      </c>
+      <c r="B19">
+        <v>229963.65</v>
+      </c>
+      <c r="C19">
+        <v>2824.5</v>
+      </c>
+      <c r="D19">
+        <v>39.6</v>
+      </c>
+      <c r="E19">
+        <v>1367.99</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>42552</v>
+      </c>
+      <c r="B20">
+        <v>166029.6</v>
+      </c>
+      <c r="C20">
+        <v>1810.2</v>
+      </c>
+      <c r="D20">
+        <v>36.9</v>
+      </c>
+      <c r="E20">
+        <v>716.06</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <v>42583</v>
+      </c>
+      <c r="B21">
+        <v>157710.45000000001</v>
+      </c>
+      <c r="C21">
+        <v>1819.65</v>
+      </c>
+      <c r="D21">
+        <v>29.7</v>
+      </c>
+      <c r="E21">
+        <v>253.89</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A22">
+        <v>42614</v>
+      </c>
+      <c r="B22">
+        <v>242557.8</v>
+      </c>
+      <c r="C22">
+        <v>2909.55</v>
+      </c>
+      <c r="D22">
+        <v>51.3</v>
+      </c>
+      <c r="E22">
+        <v>804.04</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A23">
+        <v>42644</v>
+      </c>
+      <c r="B23">
+        <v>217982.25</v>
+      </c>
+      <c r="C23">
+        <v>2885.4</v>
+      </c>
+      <c r="D23">
+        <v>31.5</v>
+      </c>
+      <c r="E23">
+        <v>173.72</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A24">
+        <v>42675</v>
+      </c>
+      <c r="B24">
+        <v>193181.55</v>
+      </c>
+      <c r="C24">
+        <v>1789.2</v>
+      </c>
+      <c r="D24">
+        <v>56.7</v>
+      </c>
+      <c r="E24">
+        <v>1355.85</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A25">
+        <v>42705</v>
+      </c>
+      <c r="B25">
+        <v>160734.29999999999</v>
+      </c>
+      <c r="C25">
+        <v>1789.2</v>
+      </c>
+      <c r="D25">
+        <v>29.7</v>
+      </c>
+      <c r="E25">
+        <v>449.11</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A26">
+        <v>42736</v>
+      </c>
+      <c r="B26">
+        <v>189872.7</v>
+      </c>
+      <c r="C26">
+        <v>2094.75</v>
+      </c>
+      <c r="D26">
+        <v>45</v>
+      </c>
+      <c r="E26">
+        <v>958.53</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A27">
+        <v>42767</v>
+      </c>
+      <c r="B27">
+        <v>180957.9</v>
+      </c>
+      <c r="C27">
+        <v>2138.85</v>
+      </c>
+      <c r="D27">
+        <v>35.1</v>
+      </c>
+      <c r="E27">
+        <v>62.69</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A28">
+        <v>42795</v>
+      </c>
+      <c r="B28">
+        <v>254835.6</v>
+      </c>
+      <c r="C28">
+        <v>2964.15</v>
+      </c>
+      <c r="D28">
+        <v>61.2</v>
+      </c>
+      <c r="E28">
+        <v>247.7</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A29">
+        <v>42826</v>
+      </c>
+      <c r="B29">
+        <v>192426.3</v>
+      </c>
+      <c r="C29">
+        <v>1849.05</v>
+      </c>
+      <c r="D29">
+        <v>61.2</v>
+      </c>
+      <c r="E29">
+        <v>124.18</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A30">
+        <v>42856</v>
+      </c>
+      <c r="B30">
+        <v>209988</v>
+      </c>
+      <c r="C30">
+        <v>2588.25</v>
+      </c>
+      <c r="D30">
+        <v>42.3</v>
+      </c>
+      <c r="E30">
+        <v>394.36</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A31">
+        <v>42887</v>
+      </c>
+      <c r="B31">
+        <v>188476.2</v>
+      </c>
+      <c r="C31">
+        <v>2175.6</v>
+      </c>
+      <c r="D31">
+        <v>35.1</v>
+      </c>
+      <c r="E31">
+        <v>247.12</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Valores preditos em R, Modelo Final, Praticando, dados fabrica
</commit_message>
<xml_diff>
--- a/dadosConnepi.xlsx
+++ b/dadosConnepi.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/b7beb5d6fee94c27/Documents/meusCursos/regressao-connepi2024Local/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="30" documentId="11_94B1572A54DEAC0FFB039038BE0E4ED8A2FF9F7C" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{965AD81C-E261-4B4E-8196-A65E7290B9A0}"/>
+  <xr:revisionPtr revIDLastSave="33" documentId="11_94B1572A54DEAC0FFB039038BE0E4ED8A2FF9F7C" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{33A7F277-941C-48E2-912B-89F4EB376EBC}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -54,7 +54,7 @@
     <t>embalagem</t>
   </si>
   <si>
-    <t>divugacao</t>
+    <t>divulgacao</t>
   </si>
 </sst>
 </file>
@@ -90,8 +90,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -539,11 +540,12 @@
   <dimension ref="A1:E31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
+    <col min="1" max="1" width="10.5546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -565,7 +567,7 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2">
+      <c r="A2" s="1">
         <v>42005</v>
       </c>
       <c r="B2">
@@ -582,7 +584,7 @@
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3">
+      <c r="A3" s="1">
         <v>42036</v>
       </c>
       <c r="B3">
@@ -599,7 +601,7 @@
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4">
+      <c r="A4" s="1">
         <v>42064</v>
       </c>
       <c r="B4">
@@ -616,7 +618,7 @@
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5">
+      <c r="A5" s="1">
         <v>42095</v>
       </c>
       <c r="B5">
@@ -633,7 +635,7 @@
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A6">
+      <c r="A6" s="1">
         <v>42125</v>
       </c>
       <c r="B6">
@@ -650,7 +652,7 @@
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A7">
+      <c r="A7" s="1">
         <v>42156</v>
       </c>
       <c r="B7">
@@ -667,7 +669,7 @@
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A8">
+      <c r="A8" s="1">
         <v>42186</v>
       </c>
       <c r="B8">
@@ -684,7 +686,7 @@
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A9">
+      <c r="A9" s="1">
         <v>42217</v>
       </c>
       <c r="B9">
@@ -701,7 +703,7 @@
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A10">
+      <c r="A10" s="1">
         <v>42248</v>
       </c>
       <c r="B10">
@@ -718,7 +720,7 @@
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A11">
+      <c r="A11" s="1">
         <v>42278</v>
       </c>
       <c r="B11">
@@ -735,7 +737,7 @@
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A12">
+      <c r="A12" s="1">
         <v>42309</v>
       </c>
       <c r="B12">
@@ -752,7 +754,7 @@
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A13">
+      <c r="A13" s="1">
         <v>42339</v>
       </c>
       <c r="B13">
@@ -769,7 +771,7 @@
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A14">
+      <c r="A14" s="1">
         <v>42370</v>
       </c>
       <c r="B14">
@@ -786,7 +788,7 @@
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A15">
+      <c r="A15" s="1">
         <v>42401</v>
       </c>
       <c r="B15">
@@ -803,7 +805,7 @@
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A16">
+      <c r="A16" s="1">
         <v>42430</v>
       </c>
       <c r="B16">
@@ -820,7 +822,7 @@
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A17">
+      <c r="A17" s="1">
         <v>42461</v>
       </c>
       <c r="B17">
@@ -837,7 +839,7 @@
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A18">
+      <c r="A18" s="1">
         <v>42491</v>
       </c>
       <c r="B18">
@@ -854,7 +856,7 @@
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A19">
+      <c r="A19" s="1">
         <v>42522</v>
       </c>
       <c r="B19">
@@ -871,7 +873,7 @@
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A20">
+      <c r="A20" s="1">
         <v>42552</v>
       </c>
       <c r="B20">
@@ -888,7 +890,7 @@
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A21">
+      <c r="A21" s="1">
         <v>42583</v>
       </c>
       <c r="B21">
@@ -905,7 +907,7 @@
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A22">
+      <c r="A22" s="1">
         <v>42614</v>
       </c>
       <c r="B22">
@@ -922,7 +924,7 @@
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A23">
+      <c r="A23" s="1">
         <v>42644</v>
       </c>
       <c r="B23">
@@ -939,7 +941,7 @@
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A24">
+      <c r="A24" s="1">
         <v>42675</v>
       </c>
       <c r="B24">
@@ -956,7 +958,7 @@
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A25">
+      <c r="A25" s="1">
         <v>42705</v>
       </c>
       <c r="B25">
@@ -973,7 +975,7 @@
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A26">
+      <c r="A26" s="1">
         <v>42736</v>
       </c>
       <c r="B26">
@@ -990,7 +992,7 @@
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A27">
+      <c r="A27" s="1">
         <v>42767</v>
       </c>
       <c r="B27">
@@ -1007,7 +1009,7 @@
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A28">
+      <c r="A28" s="1">
         <v>42795</v>
       </c>
       <c r="B28">
@@ -1024,7 +1026,7 @@
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A29">
+      <c r="A29" s="1">
         <v>42826</v>
       </c>
       <c r="B29">
@@ -1041,7 +1043,7 @@
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A30">
+      <c r="A30" s="1">
         <v>42856</v>
       </c>
       <c r="B30">
@@ -1058,7 +1060,7 @@
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A31">
+      <c r="A31" s="1">
         <v>42887</v>
       </c>
       <c r="B31">

</xml_diff>